<commit_message>
switched red and white LEDs - red is now power
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37040" windowHeight="24540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="258">
   <si>
     <t>Reference</t>
   </si>
@@ -833,6 +833,9 @@
   </si>
   <si>
     <t>296-21931-1-ND</t>
+  </si>
+  <si>
+    <t>IC10, IC11</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1642,7 +1645,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>128</v>
@@ -1822,7 +1825,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>257</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>128</v>
@@ -2176,7 +2179,7 @@
     </row>
     <row r="19" spans="1:13" ht="30">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
updated BOM to used JST through-hole connector for sync; fixed bottomlayer trace widths and routing
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="6" r:id="rId1"/>
-    <sheet name="Cost Estimator" sheetId="5" r:id="rId2"/>
-    <sheet name="Stats" sheetId="7" r:id="rId3"/>
-    <sheet name="SandSquid1" sheetId="8" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId5"/>
-    <sheet name="Manufacturing" sheetId="15" r:id="rId6"/>
-    <sheet name="Place" sheetId="16" r:id="rId7"/>
+    <sheet name="BOM Extras" sheetId="17" r:id="rId2"/>
+    <sheet name="Cost Estimator" sheetId="5" r:id="rId3"/>
+    <sheet name="Stats" sheetId="7" r:id="rId4"/>
+    <sheet name="SandSquid1" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId6"/>
+    <sheet name="Manufacturing" sheetId="15" r:id="rId7"/>
+    <sheet name="Place" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="ADS1299_shield_1.0_final" localSheetId="3">SandSquid1!$A$1:$D$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">Place!$A$1:$K$19</definedName>
+    <definedName name="ADS1299_shield_1.0_final" localSheetId="4">SandSquid1!$A$1:$D$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">Place!$A$1:$K$19</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="259">
   <si>
     <t>Reference</t>
   </si>
@@ -817,9 +818,6 @@
     <t>C7,C9,C11,C13,C15,C18,C19,C21,C22,C23,C26,C29,C30,C32,C50,C51,C52,C54,C56,C58,C60,C61,C65,C68,C70,C72</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/S3B-PH-SM4-TB(LF)(SN)/455-1750-1-ND/926847</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/MLZ2012A3R3W/445-6394-1-ND/2465720</t>
   </si>
   <si>
@@ -836,6 +834,12 @@
   </si>
   <si>
     <t>IC10, IC11</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?vendor=0&amp;keywords=%09455-1720-ND</t>
+  </si>
+  <si>
+    <t>JST_3PIN - PH Series - through hole, right angle</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1516,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1825,7 +1829,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>128</v>
@@ -1870,10 +1874,10 @@
         <v>166</v>
       </c>
       <c r="E10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" t="s">
         <v>255</v>
-      </c>
-      <c r="F10" t="s">
-        <v>256</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1886,10 +1890,10 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
+        <v>252</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2105,7 +2109,7 @@
         <v>26</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2171,10 +2175,10 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>188</v>
+        <v>258</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30">
@@ -2825,6 +2829,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="53.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="46.83203125" customWidth="1"/>
+    <col min="11" max="12" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="D3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="D9" s="9"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="D10"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="D11"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20"/>
+      <c r="D20"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="D21"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="D22"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="D23"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="D24"/>
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="D25"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="D26"/>
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="D27"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="D28"/>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="D29"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="D32"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="D33"/>
+      <c r="M33" s="3"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="M34" s="3"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="6"/>
+      <c r="B46" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -3095,7 +3336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -3189,7 +3430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -3494,7 +3735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -3883,7 +4124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -3996,7 +4237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
no changes to bom, playing with manufacturing estimator
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="6" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1015,6 +1015,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1159,7 +1160,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="86">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1240,6 +1241,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1579,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:N34"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2994,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3234,6 +3236,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
BOM updates fixing place sheet after building rev 1.1 - to match BOM sheet
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="273">
   <si>
     <t>Reference</t>
   </si>
@@ -875,6 +875,15 @@
   </si>
   <si>
     <t>VSOP8</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Microchip-Technology/24AA256-I-SN/?qs=sGAEpiMZZMuVhdAcoizlRbwEyZ%252bZRHI58GqgwuNvwSM%3d</t>
+  </si>
+  <si>
+    <t>Check orientation! Anode mark is toward ADS1299!</t>
+  </si>
+  <si>
+    <t>Check orientation! Cathode mark is away from ADS1299!</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:L37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1834,7 +1843,9 @@
       <c r="K5" t="s">
         <v>257</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
@@ -1997,7 +2008,7 @@
         <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>181</v>
+        <v>269</v>
       </c>
       <c r="D10" t="s">
         <v>164</v>
@@ -2107,7 +2118,7 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2146,7 +2157,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2184,8 +2195,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
+    <row r="15" spans="1:13" ht="30">
+      <c r="A15" s="2" t="s">
         <v>248</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2376,8 +2387,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
+    <row r="20" spans="1:13" ht="30">
+      <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3025,9 +3036,10 @@
     <hyperlink ref="M25" r:id="rId26"/>
     <hyperlink ref="M34" r:id="rId27"/>
     <hyperlink ref="M14" r:id="rId28"/>
+    <hyperlink ref="M4" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="72" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -4469,8 +4481,8 @@
   </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4873,7 +4885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:9" s="17" customFormat="1">
+    <row r="17" spans="2:10" s="17" customFormat="1">
       <c r="B17" s="21">
         <v>14</v>
       </c>
@@ -4899,7 +4911,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="29" customFormat="1">
+    <row r="18" spans="2:10" s="29" customFormat="1">
       <c r="B18" s="30">
         <v>15</v>
       </c>
@@ -4925,7 +4937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="17" customFormat="1">
+    <row r="19" spans="2:10" s="17" customFormat="1">
       <c r="B19" s="21">
         <v>16</v>
       </c>
@@ -4951,7 +4963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="29" customFormat="1">
+    <row r="20" spans="2:10" s="29" customFormat="1">
       <c r="B20" s="30">
         <v>17</v>
       </c>
@@ -4976,8 +4988,11 @@
       <c r="I20" s="29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" s="17" customFormat="1">
+      <c r="J20" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" s="17" customFormat="1">
       <c r="B21" s="21">
         <v>18</v>
       </c>
@@ -5003,7 +5018,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="29" customFormat="1">
+    <row r="22" spans="2:10" s="29" customFormat="1">
       <c r="B22" s="30">
         <v>19</v>
       </c>
@@ -5029,7 +5044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="17" customFormat="1">
+    <row r="23" spans="2:10" s="17" customFormat="1">
       <c r="B23" s="21">
         <v>20</v>
       </c>
@@ -5054,8 +5069,11 @@
       <c r="I23" s="17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" s="29" customFormat="1">
+      <c r="J23" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" s="29" customFormat="1">
       <c r="B24" s="30">
         <v>21</v>
       </c>
@@ -5081,7 +5099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="17" customFormat="1">
+    <row r="25" spans="2:10" s="17" customFormat="1">
       <c r="B25" s="21">
         <v>22</v>
       </c>
@@ -5107,7 +5125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:9" s="29" customFormat="1">
+    <row r="26" spans="2:10" s="29" customFormat="1">
       <c r="B26" s="30">
         <v>23</v>
       </c>
@@ -5133,7 +5151,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="2:9" s="17" customFormat="1">
+    <row r="27" spans="2:10" s="17" customFormat="1">
       <c r="B27" s="21">
         <v>24</v>
       </c>
@@ -5157,7 +5175,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:9" s="29" customFormat="1">
+    <row r="28" spans="2:10" s="29" customFormat="1">
       <c r="B28" s="30">
         <v>25</v>
       </c>
@@ -5181,7 +5199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:9" s="17" customFormat="1" ht="30">
+    <row r="29" spans="2:10" s="17" customFormat="1" ht="30">
       <c r="B29" s="21">
         <v>26</v>
       </c>
@@ -5203,7 +5221,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="29" customFormat="1">
+    <row r="30" spans="2:10" s="29" customFormat="1">
       <c r="B30" s="30">
         <v>27</v>
       </c>
@@ -5225,7 +5243,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="2:9" s="17" customFormat="1">
+    <row r="31" spans="2:10" s="17" customFormat="1">
       <c r="B31" s="21">
         <v>28</v>
       </c>
@@ -5246,7 +5264,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="2:9" s="29" customFormat="1">
+    <row r="32" spans="2:10" s="29" customFormat="1">
       <c r="B32" s="30">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
updated IC10,11 names and package TSSOP20 on place sheet
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="274">
   <si>
     <t>Reference</t>
   </si>
@@ -884,6 +884,9 @@
   </si>
   <si>
     <t>Check orientation! Cathode mark is away from ADS1299!</t>
+  </si>
+  <si>
+    <t>TSSOP20</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1970,6 +1973,9 @@
       </c>
       <c r="B9" s="2" t="s">
         <v>126</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>164</v>
@@ -4481,8 +4487,8 @@
   </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4707,12 +4713,14 @@
         <v>7</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="D10" s="30">
         <v>2</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="F10" s="31" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
changed TXS0102DCTR to TXS0102DCUR on place sheet
</commit_message>
<xml_diff>
--- a/cam/hackeeg-shield.xlsx
+++ b/cam/hackeeg-shield.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="273">
   <si>
     <t>Reference</t>
   </si>
@@ -515,9 +515,6 @@
   </si>
   <si>
     <t>OPA376AIDBVT</t>
-  </si>
-  <si>
-    <t>TXS0102DCTR</t>
   </si>
   <si>
     <t>S3B-PH-K-S(LF)(SN)</t>
@@ -1658,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>69</v>
@@ -1673,7 +1670,7 @@
         <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
         <v>128</v>
@@ -1685,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L1" t="s">
         <v>62</v>
@@ -1696,7 +1693,7 @@
     </row>
     <row r="2" spans="1:13" ht="45">
       <c r="A2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>126</v>
@@ -1727,7 +1724,7 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>52</v>
@@ -1735,7 +1732,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>126</v>
@@ -1747,10 +1744,10 @@
         <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1766,10 +1763,10 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1805,7 +1802,7 @@
         <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>83</v>
@@ -1819,7 +1816,7 @@
         <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>144</v>
@@ -1844,10 +1841,10 @@
         <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1858,10 +1855,10 @@
         <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>148</v>
@@ -1883,7 +1880,7 @@
         <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>108</v>
@@ -1897,10 +1894,10 @@
         <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>145</v>
@@ -1922,7 +1919,7 @@
         <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>102</v>
@@ -1936,10 +1933,10 @@
         <v>126</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>146</v>
@@ -1961,7 +1958,7 @@
         <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>104</v>
@@ -1969,19 +1966,19 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
         <v>113</v>
@@ -2000,7 +1997,7 @@
         <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>114</v>
@@ -2014,16 +2011,16 @@
         <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" t="s">
         <v>252</v>
-      </c>
-      <c r="F10" t="s">
-        <v>253</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2036,13 +2033,13 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" t="s">
+        <v>259</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="K10" t="s">
-        <v>260</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2053,10 +2050,10 @@
         <v>126</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" t="s">
         <v>149</v>
@@ -2078,7 +2075,7 @@
         <v>111</v>
       </c>
       <c r="K11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>110</v>
@@ -2092,13 +2089,13 @@
         <v>126</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>99</v>
@@ -2114,10 +2111,10 @@
         <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>100</v>
@@ -2125,7 +2122,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>126</v>
@@ -2156,7 +2153,7 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>58</v>
@@ -2164,7 +2161,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>126</v>
@@ -2176,10 +2173,10 @@
         <v>138</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -2192,18 +2189,18 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30">
       <c r="A15" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>126</v>
@@ -2234,7 +2231,7 @@
         <v>9</v>
       </c>
       <c r="K15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>56</v>
@@ -2248,16 +2245,16 @@
         <v>126</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -2273,15 +2270,15 @@
         <v>25</v>
       </c>
       <c r="K16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>126</v>
@@ -2312,7 +2309,7 @@
         <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>54</v>
@@ -2326,10 +2323,10 @@
         <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>85</v>
@@ -2345,13 +2342,13 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30">
@@ -2387,7 +2384,7 @@
         <v>77</v>
       </c>
       <c r="K19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>80</v>
@@ -2426,7 +2423,7 @@
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L20" t="s">
         <v>74</v>
@@ -2440,13 +2437,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" t="s">
         <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>156</v>
       </c>
       <c r="F21" t="s">
         <v>121</v>
@@ -2465,7 +2462,7 @@
         <v>59</v>
       </c>
       <c r="K21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>120</v>
@@ -2476,13 +2473,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" t="s">
         <v>119</v>
@@ -2498,10 +2495,10 @@
         <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>118</v>
@@ -2512,16 +2509,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2534,13 +2531,13 @@
         <v>20</v>
       </c>
       <c r="J23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2548,16 +2545,16 @@
         <v>91</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -2573,10 +2570,10 @@
         <v>61</v>
       </c>
       <c r="K24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2590,10 +2587,10 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" t="s">
         <v>159</v>
-      </c>
-      <c r="E25" t="s">
-        <v>160</v>
       </c>
       <c r="F25" t="s">
         <v>89</v>
@@ -2612,7 +2609,7 @@
         <v>29</v>
       </c>
       <c r="K25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>90</v>
@@ -2629,10 +2626,10 @@
         <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" t="s">
         <v>93</v>
@@ -2651,7 +2648,7 @@
         <v>31</v>
       </c>
       <c r="K26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>94</v>
@@ -2668,10 +2665,10 @@
         <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F27" t="s">
         <v>95</v>
@@ -2690,7 +2687,7 @@
         <v>27</v>
       </c>
       <c r="K27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>96</v>
@@ -2698,7 +2695,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>126</v>
@@ -2707,13 +2704,13 @@
         <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2726,13 +2723,13 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
+        <v>189</v>
+      </c>
+      <c r="K28" t="s">
+        <v>259</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="K28" t="s">
-        <v>260</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30">
@@ -2746,10 +2743,10 @@
         <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F29" t="s">
         <v>88</v>
@@ -2768,7 +2765,7 @@
         <v>33</v>
       </c>
       <c r="K29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>87</v>
@@ -2779,13 +2776,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>116</v>
@@ -2804,7 +2801,7 @@
         <v>60</v>
       </c>
       <c r="K30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>117</v>
@@ -2815,7 +2812,7 @@
         <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>64</v>
@@ -2838,7 +2835,7 @@
         <v>86</v>
       </c>
       <c r="K31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>122</v>
@@ -2849,7 +2846,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" t="s">
         <v>64</v>
@@ -2869,10 +2866,10 @@
         <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>123</v>
@@ -2880,10 +2877,10 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
@@ -2902,13 +2899,13 @@
         <v>36</v>
       </c>
       <c r="J33" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" t="s">
+        <v>257</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="K33" t="s">
-        <v>258</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2916,7 +2913,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>64</v>
@@ -2938,10 +2935,10 @@
         <v>35</v>
       </c>
       <c r="K34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2955,7 +2952,7 @@
         <v>37</v>
       </c>
       <c r="K35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L35" t="s">
         <v>97</v>
@@ -2972,7 +2969,7 @@
         <v>39</v>
       </c>
       <c r="K36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L36" t="s">
         <v>97</v>
@@ -2989,7 +2986,7 @@
         <v>41</v>
       </c>
       <c r="K37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L37" t="s">
         <v>97</v>
@@ -3079,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>69</v>
@@ -3094,7 +3091,7 @@
         <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
         <v>128</v>
@@ -3109,7 +3106,7 @@
         <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M1" t="s">
         <v>51</v>
@@ -3117,22 +3114,22 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="D2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="J2" t="s">
         <v>265</v>
       </c>
-      <c r="J2" t="s">
-        <v>266</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -3338,19 +3335,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" t="s">
         <v>235</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>236</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>237</v>
-      </c>
-      <c r="F4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3435,7 +3432,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -3480,7 +3477,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -3500,7 +3497,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="10">
         <f>B11+B11*B15</f>
@@ -3525,7 +3522,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -3545,7 +3542,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20">
         <f>B17+B17*B18</f>
@@ -3622,13 +3619,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" s="8">
         <v>148</v>
@@ -3636,7 +3633,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="8">
         <v>115</v>
@@ -3644,7 +3641,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9">
         <f>COUNT(BOM!G2:G37)</f>
@@ -3653,7 +3650,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10">
         <f>SUM(BOM!G2:G38)</f>
@@ -3705,7 +3702,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -3716,7 +3713,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3727,7 +3724,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -3738,13 +3735,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>195</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3760,7 +3757,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -3771,7 +3768,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -3788,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3799,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3810,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3821,7 +3818,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3832,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3843,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3854,7 +3851,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3865,7 +3862,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3876,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3887,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3947,13 +3944,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3964,7 +3961,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3993,7 +3990,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -4013,10 +4010,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D30" si="0">IF(A3=C3, "equal", "not")</f>
@@ -4145,10 +4142,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -4253,10 +4250,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -4313,10 +4310,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -4382,20 +4379,20 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="C2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" t="s">
         <v>230</v>
-      </c>
-      <c r="G2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -4418,7 +4415,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" s="12">
         <v>650</v>
@@ -4447,7 +4444,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -4488,7 +4485,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4506,7 +4503,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="13" customFormat="1" ht="23">
       <c r="A1" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="14"/>
@@ -4522,16 +4519,16 @@
     </row>
     <row r="3" spans="1:10" s="22" customFormat="1">
       <c r="A3" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>240</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>69</v>
@@ -4563,19 +4560,19 @@
         <v>1</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H4" s="31" t="s">
         <v>99</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="17" customFormat="1">
@@ -4589,13 +4586,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>150</v>
+        <v>251</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>112</v>
@@ -4615,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>144</v>
@@ -4641,10 +4638,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>148</v>
@@ -4667,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>145</v>
@@ -4693,10 +4690,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>146</v>
@@ -4713,19 +4710,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="30">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>113</v>
@@ -4745,10 +4742,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>149</v>
@@ -4765,7 +4762,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D12" s="30">
         <v>26</v>
@@ -4829,10 +4826,10 @@
         <v>70</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>88</v>
@@ -4846,7 +4843,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" s="21">
         <v>13</v>
@@ -4872,7 +4869,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="30">
         <v>8</v>
@@ -4907,10 +4904,10 @@
         <v>70</v>
       </c>
       <c r="F17" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>160</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>89</v>
@@ -4924,7 +4921,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" s="30">
         <v>3</v>
@@ -4950,7 +4947,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" s="21">
         <v>2</v>
@@ -4962,10 +4959,10 @@
         <v>132</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>5</v>
@@ -4997,7 +4994,7 @@
         <v>82</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="17" customFormat="1">
@@ -5005,7 +5002,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D21" s="21">
         <v>2</v>
@@ -5017,13 +5014,13 @@
         <v>138</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="2:10" s="29" customFormat="1">
@@ -5043,7 +5040,7 @@
         <v>134</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>98</v>
@@ -5078,7 +5075,7 @@
         <v>77</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="2:10" s="29" customFormat="1">
@@ -5095,10 +5092,10 @@
         <v>70</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>93</v>
@@ -5121,10 +5118,10 @@
         <v>70</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>95</v>
@@ -5138,7 +5135,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D26" s="30">
         <v>1</v>
@@ -5147,16 +5144,16 @@
         <v>70</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H26" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="I26" s="29" t="s">
         <v>189</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="27" spans="2:10" s="17" customFormat="1">
@@ -5171,13 +5168,13 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>61</v>
@@ -5198,7 +5195,7 @@
         <v>115</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H28" s="31" t="s">
         <v>116</v>
@@ -5248,7 +5245,7 @@
       </c>
       <c r="H30" s="31"/>
       <c r="I30" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="2:10" s="17" customFormat="1">
@@ -5256,7 +5253,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D31" s="21">
         <v>1</v>
@@ -5269,7 +5266,7 @@
         <v>19950</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="2:10" s="29" customFormat="1">
@@ -5305,10 +5302,10 @@
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>155</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>121</v>
@@ -5329,16 +5326,16 @@
       </c>
       <c r="E34" s="31"/>
       <c r="F34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H34" s="29" t="s">
         <v>119</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="17" customFormat="1">
@@ -5353,16 +5350,16 @@
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="2:9" s="29" customFormat="1">
@@ -5377,16 +5374,16 @@
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H36" s="31" t="s">
         <v>85</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="29" customFormat="1">
@@ -5446,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>69</v>
@@ -5461,7 +5458,7 @@
         <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
         <v>128</v>
@@ -5476,7 +5473,7 @@
         <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M1" t="s">
         <v>51</v>
@@ -5484,7 +5481,7 @@
     </row>
     <row r="2" spans="1:13" ht="45">
       <c r="A2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>126</v>
@@ -5515,7 +5512,7 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>52</v>
@@ -5523,7 +5520,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>126</v>
@@ -5535,10 +5532,10 @@
         <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -5554,7 +5551,7 @@
         <v>5</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -5601,10 +5598,10 @@
         <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>148</v>
@@ -5637,10 +5634,10 @@
         <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>145</v>
@@ -5673,10 +5670,10 @@
         <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>146</v>
@@ -5703,16 +5700,16 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
         <v>113</v>
@@ -5742,16 +5739,16 @@
         <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F9" t="s">
         <v>252</v>
-      </c>
-      <c r="F9" t="s">
-        <v>253</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -5764,10 +5761,10 @@
         <v>8</v>
       </c>
       <c r="J9" t="s">
+        <v>249</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -5778,10 +5775,10 @@
         <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
         <v>149</v>
@@ -5814,13 +5811,13 @@
         <v>126</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>99</v>
@@ -5836,7 +5833,7 @@
         <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>100</v>
@@ -5844,7 +5841,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>126</v>
@@ -5880,7 +5877,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>126</v>
@@ -5892,10 +5889,10 @@
         <v>138</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -5908,15 +5905,15 @@
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>126</v>
@@ -5958,16 +5955,16 @@
         <v>126</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -5983,12 +5980,12 @@
         <v>25</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>126</v>
@@ -6030,13 +6027,13 @@
         <v>126</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -6049,10 +6046,10 @@
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="30">
@@ -6135,13 +6132,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" t="s">
         <v>155</v>
-      </c>
-      <c r="E20" t="s">
-        <v>156</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
@@ -6168,13 +6165,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F21" t="s">
         <v>119</v>
@@ -6190,7 +6187,7 @@
         <v>8</v>
       </c>
       <c r="J21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>118</v>
@@ -6201,16 +6198,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -6223,10 +6220,10 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -6234,16 +6231,16 @@
         <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G23">
         <v>5</v>
@@ -6259,7 +6256,7 @@
         <v>61</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -6273,10 +6270,10 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" t="s">
         <v>159</v>
-      </c>
-      <c r="E24" t="s">
-        <v>160</v>
       </c>
       <c r="F24" t="s">
         <v>89</v>
@@ -6309,10 +6306,10 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F25" t="s">
         <v>93</v>
@@ -6345,10 +6342,10 @@
         <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F26" t="s">
         <v>95</v>
@@ -6372,7 +6369,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>126</v>
@@ -6381,13 +6378,13 @@
         <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -6400,10 +6397,10 @@
         <v>2</v>
       </c>
       <c r="J27" t="s">
+        <v>189</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30">
@@ -6417,10 +6414,10 @@
         <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F28" t="s">
         <v>88</v>
@@ -6447,13 +6444,13 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>116</v>

</xml_diff>